<commit_message>
inklusive csv speed vs. accuracy
</commit_message>
<xml_diff>
--- a/exp/stroop/stroop_condition_file_practice.xlsx
+++ b/exp/stroop/stroop_condition_file_practice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unibe365-my.sharepoint.com/personal/rebekka_borer_unibe_ch/Documents/HILFSASSISTENZ/Computerlab/psychopy/stroop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\neuroscicomplabFS24\exp\stroop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{6F73DED9-5CBE-4F6F-B86E-324F47B9B339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3B32B1D-7A38-4597-9432-4D070176B151}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9936571E-33C0-46C9-8130-4A72010C104F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13125" yWindow="630" windowWidth="13815" windowHeight="16440" xr2:uid="{4C46569A-3757-4893-A4D0-58B4E06493E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{4C46569A-3757-4893-A4D0-58B4E06493E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
   <si>
     <t>red</t>
   </si>
@@ -141,10 +141,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B945B772-D172-4BF6-B00C-526EBD24F003}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,17 +480,17 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -502,10 +498,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -513,13 +509,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -529,14 +525,14 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,54 +540,96 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
     </row>

</xml_diff>